<commit_message>
study, study type, breed, diagnosis, stg of dis, total 67 test scripts to jenkins
</commit_message>
<xml_diff>
--- a/InputFiles/TC33_Canine_Filter_Breed-Labrador.xlsx
+++ b/InputFiles/TC33_Canine_Filter_Breed-Labrador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7963150-B4E2-4AEF-88EE-4796210D2516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2B2042-4DCC-4209-816B-9A82BE4D64EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="10" windowWidth="19200" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Labrador Retriever']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 WHERE demo.breed IN ['Labrador Retriever']
 MATCH (c)&lt;--(diag:diagnosis)
@@ -121,6 +118,22 @@
   </si>
   <si>
     <t>TC33_Canine_Filter_Breed-Labrador_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)
+  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
+  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
+  MATCH (d:diagnosis)
+  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
+  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+    WHERE demo.breed IN ['Labrador Retriever']
+  OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+  OPTIONAL MATCH (samp:sample)-[*]-&gt;(c)
+  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
+  RETURN count(DISTINCT(f)) as number_of_files ,
+             count(DISTINCT(samp)) as number_of_sample ,
+             count(DISTINCT(c.case_id)) as number_of_cases ,
+             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
 </sst>
 </file>
@@ -492,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,33 +539,33 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
@@ -560,16 +573,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>